<commit_message>
added info exclusion criteria
</commit_message>
<xml_diff>
--- a/Mental Health Products.xlsx
+++ b/Mental Health Products.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annekleine/Dropbox/Human_AI/Mental_heal/MentalHealth_AI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AFE61E-A4F5-8046-B0E9-1E7FC1F036A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A345EE-A411-0E4C-A5E9-AE0D186182AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14300" windowHeight="16280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="13880" windowHeight="16360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <author>Anka K</author>
   </authors>
   <commentList>
-    <comment ref="AW1" authorId="0" shapeId="0" xr:uid="{8A334D93-AE1A-614A-AB5D-88791A4E2502}">
+    <comment ref="BD1" authorId="0" shapeId="0" xr:uid="{BEA0A380-500C-BE4C-A1D8-BD2A11368CFE}">
       <text>
         <r>
           <rPr>
@@ -56,11 +56,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>QUADAS-2 criteria</t>
+          <t>See here https://www.bmj.com/content/375/bmj.n2281 and here https://www.probast.org/wp-content/uploads/2020/02/PROBAST_20190515.pdf and here https://www.probast.org/wp-content/uploads/2020/02/aime201901010-m181377.pdf</t>
         </r>
       </text>
     </comment>
-    <comment ref="BB1" authorId="0" shapeId="0" xr:uid="{DE7ACCB0-AA16-FE44-AF9C-0F462A715127}">
+    <comment ref="CD2" authorId="0" shapeId="0" xr:uid="{DE7ACCB0-AA16-FE44-AF9C-0F462A715127}">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{64B70843-A1EF-5C4A-BA58-43BA23E2704B}">
+    <comment ref="P4" authorId="0" shapeId="0" xr:uid="{F552E3A2-2445-8F44-9563-9CBE4EC9AFC3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anka K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>819,951 (573,965 training; 1782 suicide deaths) (245,986 testing; 764 suicide deaths)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T4" authorId="0" shapeId="0" xr:uid="{64B70843-A1EF-5C4A-BA58-43BA23E2704B}">
       <text>
         <r>
           <rPr>
@@ -126,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P3" authorId="0" shapeId="0" xr:uid="{F552E3A2-2445-8F44-9563-9CBE4EC9AFC3}">
+    <comment ref="BD9" authorId="0" shapeId="0" xr:uid="{DDBA8A92-9B19-9D40-88DA-A4BC65E12CCE}">
       <text>
         <r>
           <rPr>
@@ -155,7 +188,311 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>819,951 (573,965 training; 1782 suicide deaths) (245,986 testing; 764 suicide deaths)</t>
+          <t>Yes, nested case control</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BI11" authorId="0" shapeId="0" xr:uid="{9C3DDFF6-5E18-E741-AEB4-396D1729E832}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anka K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">because outcomes assessed </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BM11" authorId="0" shapeId="0" xr:uid="{ADCE7709-A321-B343-A0A4-03D1C52B5FA1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anka K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>yes because health care professional assessed ASD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BN11" authorId="0" shapeId="0" xr:uid="{0576EAE8-CAC2-B34F-90D3-9A242C269D30}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anka K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">yes because based on DSM </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BQ11" authorId="0" shapeId="0" xr:uid="{CA50E19E-EA66-A64A-92B9-BB5997804E15}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anka K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Yes, because MRI independent of ASD assessment </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BU11" authorId="0" shapeId="0" xr:uid="{8ED4DCEF-DECF-004C-8B17-254FEF4D36C1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anka K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">No, because </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>the number of participants with the outcome relative to the number of candidate predictor parameters was</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> not</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve"> ≥20 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="BZ11" authorId="0" shapeId="0" xr:uid="{06F81320-5922-2F47-9911-79D32B601AF3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anka K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Yes, because nested case control with qual group size </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CA11" authorId="0" shapeId="0" xr:uid="{5D139308-BF3E-054B-A2B8-FD08417A6349}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anka K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">No because </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>classification measures (like sensitivity, specificity, or predictive values) were presented using predicted probability thresholds derived from the data set at hand.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="CB11" authorId="0" shapeId="0" xr:uid="{B154A12F-974B-804D-A1D7-E6D6D49D17B9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Anka K:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Yes, because cross validation was used </t>
         </r>
       </text>
     </comment>
@@ -164,7 +501,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="511">
   <si>
     <t>Firm</t>
   </si>
@@ -992,27 +1329,18 @@
     <t>Availability</t>
   </si>
   <si>
-    <t>Primary goal</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
     <t>Age Range</t>
   </si>
   <si>
-    <t>AI Method</t>
-  </si>
-  <si>
     <t>Validation type</t>
   </si>
   <si>
     <t>Conclusion</t>
   </si>
   <si>
-    <t>Contact Info</t>
-  </si>
-  <si>
     <t>Product info in article</t>
   </si>
   <si>
@@ -1094,15 +1422,9 @@
     <t>Graham, S., Depp, C., Lee, E. E., Nebeker, C., Tu, X., Kim, H. C., &amp; Jeste, D. V. (2019). Artificial intelligence for mental health and mental illnesses: an overview. Current psychiatry reports, 21(11), 1-18</t>
   </si>
   <si>
-    <t>Graham et al., 2019</t>
-  </si>
-  <si>
     <t>Arun, V., Prajwal, V., Krishna, M., Arunkumar, B. V., Padma, S. K., &amp; Shyam, V. (2018, November). A boosted machine learning approach for detection of depression. In 2018 IEEE Symposium Series on Computational Intelligence (SSCI) (pp. 41-47). IEEE.</t>
   </si>
   <si>
-    <t>Arun et al., 2018</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -1127,9 +1449,6 @@
     <t>vanishriarun@sjce.ac.in</t>
   </si>
   <si>
-    <t>Choi et al., 2018</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -1154,48 +1473,6 @@
     <t xml:space="preserve">Year of publication </t>
   </si>
   <si>
-    <t>Sample Size model development</t>
-  </si>
-  <si>
-    <t>Subjects model development</t>
-  </si>
-  <si>
-    <t>Number of folds</t>
-  </si>
-  <si>
-    <t>Domains risk of bias (limitations)</t>
-  </si>
-  <si>
-    <t>Indirectness of patient setting</t>
-  </si>
-  <si>
-    <t>Indirectness of outcome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inconsistency </t>
-  </si>
-  <si>
-    <t>Imprecision</t>
-  </si>
-  <si>
-    <t>Overall quality of evidence</t>
-  </si>
-  <si>
-    <t>Patient selection</t>
-  </si>
-  <si>
-    <t>Index test</t>
-  </si>
-  <si>
-    <t>Reference standard</t>
-  </si>
-  <si>
-    <t>Flow and timing</t>
-  </si>
-  <si>
-    <t>Data management</t>
-  </si>
-  <si>
     <t>PubMed</t>
   </si>
   <si>
@@ -1211,12 +1488,6 @@
     <t>Kintsugi</t>
   </si>
   <si>
-    <t>Shatte et al., 2019</t>
-  </si>
-  <si>
-    <t>Lueken et al., 2015</t>
-  </si>
-  <si>
     <t>Predict depressive comorbidity in anxiety patients</t>
   </si>
   <si>
@@ -1238,24 +1509,12 @@
     <t>Best algorithm</t>
   </si>
   <si>
-    <t>Controlled confounders</t>
-  </si>
-  <si>
-    <t>Performance confounders controlled</t>
-  </si>
-  <si>
-    <t>Data Source</t>
-  </si>
-  <si>
     <t xml:space="preserve">Germany </t>
   </si>
   <si>
     <t>Multicenter</t>
   </si>
   <si>
-    <t>Anxiety patients</t>
-  </si>
-  <si>
     <t>Unicenter</t>
   </si>
   <si>
@@ -1316,18 +1575,12 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>Not decreased</t>
-  </si>
-  <si>
     <t>Ulrike Lueken: Lueken_U@ukw.de</t>
   </si>
   <si>
     <t>Lueken, U., Straube, B., Yang, Y., Hahn, T., Beesdo-Baum, K., Wittchen, H. U., ... &amp; Kircher, T. (2015). Separating depressive comorbidity from panic disorder: a combined functional magnetic resonance imaging and machine learning approach. Journal of affective disorders, 184, 182-192.</t>
   </si>
   <si>
-    <t>Tran &amp; Kavuluru, 2017</t>
-  </si>
-  <si>
     <t>it would make it possible for physicians and other healthcare professionals to make quick assessments, based on a relatively small narrative, that could lead to early hints of a mental disorder</t>
   </si>
   <si>
@@ -1349,9 +1602,6 @@
     <t xml:space="preserve">CNN with output score thresholding </t>
   </si>
   <si>
-    <t>Zhou et al., 2015</t>
-  </si>
-  <si>
     <t xml:space="preserve">Predict depression level or suicide possibility </t>
   </si>
   <si>
@@ -1407,12 +1657,6 @@
   </si>
   <si>
     <t>Comorbidity</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Liu et al., 2015</t>
   </si>
   <si>
     <t>Differentiate anxiety patients from others</t>
@@ -1436,9 +1680,6 @@
     <t>China</t>
   </si>
   <si>
-    <t>Half depression patients, half  general</t>
-  </si>
-  <si>
     <t>MR images</t>
   </si>
   <si>
@@ -1448,12 +1689,6 @@
     <t>18-40</t>
   </si>
   <si>
-    <t xml:space="preserve">Half social anxiety patients, half general </t>
-  </si>
-  <si>
-    <t>Detailed category</t>
-  </si>
-  <si>
     <t>Differentiation healthy and ill</t>
   </si>
   <si>
@@ -1476,9 +1711,6 @@
   </si>
   <si>
     <t>148 features across the default mode network (DMN), visual network (VN), sensory-motor network (SMN), and affective network (AN)</t>
-  </si>
-  <si>
-    <t>Sample size test dataset/ control group</t>
   </si>
   <si>
     <t>SVM</t>
@@ -1515,24 +1747,12 @@
     <t>Japan</t>
   </si>
   <si>
-    <t xml:space="preserve">Subjects validation dataset/ control group </t>
-  </si>
-  <si>
-    <t>Validation dataset</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>44 ASD, 44 healthy</t>
-  </si>
-  <si>
     <t>30.7</t>
   </si>
   <si>
-    <t>Feature selection process</t>
-  </si>
-  <si>
     <t xml:space="preserve">cross validated feature selection </t>
   </si>
   <si>
@@ -1545,16 +1765,294 @@
     <t>Accuracy validation dataset</t>
   </si>
   <si>
-    <t>0.62</t>
-  </si>
-  <si>
     <t>Yahata, N., Morimoto, J., Hashimoto, R., Lisi, G., Shibata, K., Kawakubo, Y., ... &amp; Kawato, M. (2016). A small number of abnormal brain connections predicts adult autism spectrum disorder. Nature communications, 7(1), 1-12.</t>
   </si>
   <si>
-    <t xml:space="preserve">Yahata et al., 2016 </t>
-  </si>
-  <si>
-    <t>74 ASD, 107 healthy</t>
+    <t>Domain 1: Participants, A. RISK OF BIAS (low/ high/ unclear)</t>
+  </si>
+  <si>
+    <t>Domain 2: Predictors, A. RISK OF BIAS (low/ high/ unclear)</t>
+  </si>
+  <si>
+    <t>Methodological features</t>
+  </si>
+  <si>
+    <t>GS1_Shatte_2019</t>
+  </si>
+  <si>
+    <t>Lueken_2015</t>
+  </si>
+  <si>
+    <t>Tran_2017</t>
+  </si>
+  <si>
+    <t>Zhou_2015</t>
+  </si>
+  <si>
+    <t>Liu_2015</t>
+  </si>
+  <si>
+    <t>Yahata_2016</t>
+  </si>
+  <si>
+    <t>Arun_2018</t>
+  </si>
+  <si>
+    <t>Choi_2018</t>
+  </si>
+  <si>
+    <t>GS2_Graham_2019</t>
+  </si>
+  <si>
+    <t>Shatte, A. B. R., Hutchinson, D. M., &amp; Teague, S. J. (2019). Machine learning in mental health: A scoping review of methods and applications. Psychological Medicine, 49(9), 1426–1448. https://doi.org/10.1017/S0033291719000151</t>
+  </si>
+  <si>
+    <t>Primary study goal</t>
+  </si>
+  <si>
+    <t>Category - details</t>
+  </si>
+  <si>
+    <t>Sample size validation dataset</t>
+  </si>
+  <si>
+    <t>0.89</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>AUC validation dataset</t>
+  </si>
+  <si>
+    <t>Specificity validation dataset</t>
+  </si>
+  <si>
+    <t>Sensitivity validation dataset</t>
+  </si>
+  <si>
+    <t>Precision validation dataset</t>
+  </si>
+  <si>
+    <t>F! validation dataset</t>
+  </si>
+  <si>
+    <t>external validation</t>
+  </si>
+  <si>
+    <t>External validation</t>
+  </si>
+  <si>
+    <t>Multiple external validation datasets</t>
+  </si>
+  <si>
+    <t>Differentiation healthy and ADS</t>
+  </si>
+  <si>
+    <t>Data Source Training dataset</t>
+  </si>
+  <si>
+    <t>Country training dataset</t>
+  </si>
+  <si>
+    <t>Subjects training dataset: ill</t>
+  </si>
+  <si>
+    <t>Overall sample size training dataset</t>
+  </si>
+  <si>
+    <t>Subjects training dataset: comparison group</t>
+  </si>
+  <si>
+    <t>External validation dataset</t>
+  </si>
+  <si>
+    <t>Subjects validation dataset: ill</t>
+  </si>
+  <si>
+    <t>Subjects validation dataset: comparison group</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>ML Method</t>
+  </si>
+  <si>
+    <t>L1-SCCA; SLR; logistic regression</t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Concern that the included participants and setting do not match
+the review question; Domain 1: Participants, B. APPLICABILITY  (low/ high/ unclear)</t>
+  </si>
+  <si>
+    <t>Concern that the definition, assessment or timing of predictors in
+the model do not match the review question; Domain 2: Predictors, B. APPLICABILITY  (low/ high/ unclear)</t>
+  </si>
+  <si>
+    <t>3.6 Was the time interval between predictor assessment and outcome determination appropriate?</t>
+  </si>
+  <si>
+    <t>Domain 3: Outcome, A. RISK OF BIAS (low/ high/ unclear)</t>
+  </si>
+  <si>
+    <t>1.1 Were appropriate data sources used, e.g. cohort, RCT or nested case-control study
+data?</t>
+  </si>
+  <si>
+    <t>1.2 Were all inclusions and exclusions of participants appropriate?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2.1 Were predictors defined and assessed in a similar way for all participants?</t>
+  </si>
+  <si>
+    <t>2.2 Were predictor assessments made without knowledge of outcome data? (in validation)</t>
+  </si>
+  <si>
+    <t>2.3 Are all predictors available at the time the model is intended to be used?</t>
+  </si>
+  <si>
+    <t>3.1 Was the outcome determined appropriately?</t>
+  </si>
+  <si>
+    <t>3.2 Was a pre-specified or standard outcome definition used?</t>
+  </si>
+  <si>
+    <t>3.3 Were predictors excluded from the outcome definition?</t>
+  </si>
+  <si>
+    <t>3.4 Was the outcome defined and determined in a similar way for all participants?</t>
+  </si>
+  <si>
+    <t>3.5 Was the outcome determined without knowledge of predictor information?</t>
+  </si>
+  <si>
+    <t>Concern that the outcome, its definition, timing or
+determination do not match the review question; Domain 3: Outcome, B. APPLICABILITY  (low/ high/ unclear)</t>
+  </si>
+  <si>
+    <t>4.1 Were there a reasonable number of participants with the outcome?</t>
+  </si>
+  <si>
+    <t>4.2 Were continuous and categorical predictors handled appropriately?</t>
+  </si>
+  <si>
+    <t>4.3 Were all enrolled participants included in the analysis?</t>
+  </si>
+  <si>
+    <t>4.4 Were participants with missing data handled appropriately?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.5 Was selection of predictors based on univariable analysis avoided? </t>
+  </si>
+  <si>
+    <t>4.6 Were complexities in the data (e.g. censoring, competing risks, sampling of controls)
+accounted for appropriately?</t>
+  </si>
+  <si>
+    <t>4.7 Were relevant model performance measures evaluated appropriately?</t>
+  </si>
+  <si>
+    <t>4.8 Were model overfitting and optimism in model performance accounted for?</t>
+  </si>
+  <si>
+    <t>Domain 4: Analysis, A. RISK OF BIAS (low/ high/ unclear)</t>
+  </si>
+  <si>
+    <t>Study quality (PROBAST)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study characteristics </t>
+  </si>
+  <si>
+    <t>Contact information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product information </t>
+  </si>
+  <si>
+    <t>Product mentioned (either in text or in affliations, statement of conflicts)</t>
+  </si>
+  <si>
+    <t>Plitt, M., Barnes, K. A., &amp; Martin, A. (2015). Functional connectivity classification of autism identifies highly predictive brain features but falls short of biomarker standards. NeuroImage: Clinical, 7, 359–366. https://doi.org/10.1016/j.nicl.2014.12.013</t>
+  </si>
+  <si>
+    <t>Plitt_2015</t>
+  </si>
+  <si>
+    <t>determined the best methods for performing classification of ASD vs. TD participants using rs-fMRI data</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>18.3</t>
+  </si>
+  <si>
+    <t>57 features</t>
+  </si>
+  <si>
+    <t>L-SVM</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>Positive predictive value</t>
+  </si>
+  <si>
+    <t>Negative predictive value</t>
+  </si>
+  <si>
+    <t>Positive predictive value validation dataset</t>
+  </si>
+  <si>
+    <t>Negative predictive value validation dataset</t>
+  </si>
+  <si>
+    <t>70.63</t>
+  </si>
+  <si>
+    <t>70.59</t>
+  </si>
+  <si>
+    <t>accuracy achieved using simple behavior metrics, the Social Responsiveness Scale (SRS) , far exceeded accuracy achieved with rs-fMRI. Nonetheless, classification techniques applied to rs-fMRI data still had demonstrable utility. These data-driven methods identified aberrant connections in ASD participants, revealing connections within specific networks that were predictive of an ASD diagnosis and correlated with symptom expression</t>
+  </si>
+  <si>
+    <t>This approach may be well suited for predicting the trajectory of the disorder, identifying clinical subgroups on the basis of a functional connectivity phenotype, or identifying individuals who may be more responsive to treatment. Autism is a heterogeneous developmental disorder with a range of symptom expression profiles, and rs-fMRI may have a role in explicating the root of this heterogeneity.</t>
+  </si>
+  <si>
+    <t>mark.plitt@nih.gov</t>
+  </si>
+  <si>
+    <t>Percent female</t>
+  </si>
+  <si>
+    <t>Study type</t>
+  </si>
+  <si>
+    <t>Case control</t>
+  </si>
+  <si>
+    <t>Feature selection procedure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -1642,7 +2140,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1663,38 +2161,80 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEA9999"/>
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFEA9999"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA4C2F4"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FFA4C2F4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB6D7A8"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor rgb="FFB6D7A8"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor rgb="FFA4C2F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFA4C2F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor rgb="FFB6D7A8"/>
       </patternFill>
     </fill>
   </fills>
@@ -1711,7 +2251,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1730,19 +2270,35 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1964,8 +2520,8 @@
   </sheetPr>
   <dimension ref="A1:AN32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2060,7 +2616,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -2851,7 +3407,7 @@
         <v>116</v>
       </c>
       <c r="B19" s="3"/>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="18" t="s">
         <v>117</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -3201,10 +3757,10 @@
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13" t="s">
-        <v>345</v>
+        <v>325</v>
       </c>
       <c r="C32" t="s">
-        <v>344</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -3540,13 +4096,13 @@
       <c r="I7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="17" t="s">
-        <v>342</v>
+        <v>322</v>
       </c>
       <c r="M7" s="13">
         <v>6</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
@@ -3570,13 +4126,13 @@
       <c r="I8" s="13"/>
       <c r="K8" s="13"/>
       <c r="L8" s="13" t="s">
-        <v>343</v>
+        <v>323</v>
       </c>
       <c r="M8" s="13">
         <v>7</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>341</v>
+        <v>321</v>
       </c>
       <c r="O8" s="13"/>
       <c r="P8" s="13"/>
@@ -21562,1015 +22118,1658 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:CA9"/>
+  <dimension ref="A1:DC11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9"/>
+    <sheetView tabSelected="1" topLeftCell="BV1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="CC15" sqref="CC15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B1" s="32" t="s">
+        <v>419</v>
+      </c>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="30" t="s">
+        <v>482</v>
+      </c>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="35" t="s">
+        <v>483</v>
+      </c>
+      <c r="BD1" s="33" t="s">
+        <v>481</v>
+      </c>
+      <c r="BE1" s="33"/>
+      <c r="BF1" s="33"/>
+      <c r="BG1" s="33"/>
+      <c r="BH1" s="33"/>
+      <c r="BI1" s="33"/>
+      <c r="BJ1" s="33"/>
+      <c r="BK1" s="33"/>
+      <c r="BL1" s="33"/>
+      <c r="BM1" s="33"/>
+      <c r="BN1" s="33"/>
+      <c r="BO1" s="33"/>
+      <c r="BP1" s="33"/>
+      <c r="BQ1" s="33"/>
+      <c r="BR1" s="33"/>
+      <c r="BS1" s="33"/>
+      <c r="BT1" s="33"/>
+      <c r="BU1" s="33"/>
+      <c r="BV1" s="33"/>
+      <c r="BW1" s="33"/>
+      <c r="BX1" s="33"/>
+      <c r="BY1" s="33"/>
+      <c r="BZ1" s="33"/>
+      <c r="CA1" s="33"/>
+      <c r="CB1" s="33"/>
+      <c r="CC1" s="33"/>
+      <c r="CD1" s="37" t="s">
+        <v>484</v>
+      </c>
+      <c r="CE1" s="37"/>
+      <c r="CF1" s="37"/>
+      <c r="CG1" s="37"/>
+      <c r="CH1" s="37"/>
+      <c r="CI1" s="37"/>
+      <c r="CJ1" s="37"/>
+      <c r="CK1" s="37"/>
+      <c r="CL1" s="37"/>
+      <c r="CM1" s="37"/>
+      <c r="CN1" s="37"/>
+      <c r="CO1" s="37"/>
+      <c r="CP1" s="37"/>
+      <c r="CQ1" s="37"/>
+      <c r="CR1" s="37"/>
+      <c r="CS1" s="37"/>
+      <c r="CT1" s="37"/>
+      <c r="CU1" s="37"/>
+      <c r="CV1" s="37"/>
+      <c r="CW1" s="37"/>
+      <c r="CX1" s="37"/>
+      <c r="CY1" s="37"/>
+      <c r="CZ1" s="37"/>
+      <c r="DA1" s="37"/>
+      <c r="DB1" s="37"/>
+      <c r="DC1" s="37"/>
+    </row>
+    <row r="2" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B2" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C2" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D2" s="24" t="s">
         <v>270</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E2" s="24" t="s">
         <v>271</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F2" s="24" t="s">
         <v>272</v>
       </c>
-      <c r="G1" s="19" t="s">
-        <v>407</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>326</v>
-      </c>
-      <c r="I1" s="19" t="s">
+      <c r="G2" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>430</v>
+      </c>
+      <c r="J2" s="31" t="s">
+        <v>282</v>
+      </c>
+      <c r="K2" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="L2" s="31" t="s">
+        <v>431</v>
+      </c>
+      <c r="M2" s="31" t="s">
+        <v>445</v>
+      </c>
+      <c r="N2" s="31" t="s">
+        <v>446</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>448</v>
+      </c>
+      <c r="P2" s="31" t="s">
+        <v>447</v>
+      </c>
+      <c r="Q2" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="R2" s="31" t="s">
+        <v>329</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>504</v>
+      </c>
+      <c r="T2" s="31" t="s">
+        <v>444</v>
+      </c>
+      <c r="U2" s="31" t="s">
+        <v>340</v>
+      </c>
+      <c r="V2" s="31" t="s">
+        <v>366</v>
+      </c>
+      <c r="W2" s="31" t="s">
+        <v>338</v>
+      </c>
+      <c r="X2" s="31" t="s">
+        <v>505</v>
+      </c>
+      <c r="Y2" s="31" t="s">
+        <v>398</v>
+      </c>
+      <c r="Z2" s="31" t="s">
+        <v>507</v>
+      </c>
+      <c r="AA2" s="31" t="s">
+        <v>453</v>
+      </c>
+      <c r="AB2" s="31" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC2" s="31" t="s">
+        <v>449</v>
+      </c>
+      <c r="AD2" s="31" t="s">
+        <v>450</v>
+      </c>
+      <c r="AE2" s="31" t="s">
+        <v>451</v>
+      </c>
+      <c r="AF2" s="31" t="s">
+        <v>432</v>
+      </c>
+      <c r="AG2" s="31" t="s">
+        <v>332</v>
+      </c>
+      <c r="AH2" s="31" t="s">
+        <v>343</v>
+      </c>
+      <c r="AI2" s="31" t="s">
+        <v>344</v>
+      </c>
+      <c r="AJ2" s="31" t="s">
+        <v>345</v>
+      </c>
+      <c r="AK2" s="31" t="s">
+        <v>373</v>
+      </c>
+      <c r="AL2" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="AM2" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="AN2" s="31" t="s">
+        <v>495</v>
+      </c>
+      <c r="AO2" s="31" t="s">
+        <v>496</v>
+      </c>
+      <c r="AP2" s="31" t="s">
+        <v>441</v>
+      </c>
+      <c r="AQ2" s="31" t="s">
+        <v>442</v>
+      </c>
+      <c r="AR2" s="31" t="s">
+        <v>415</v>
+      </c>
+      <c r="AS2" s="31" t="s">
+        <v>436</v>
+      </c>
+      <c r="AT2" s="31" t="s">
+        <v>437</v>
+      </c>
+      <c r="AU2" s="31" t="s">
+        <v>438</v>
+      </c>
+      <c r="AV2" s="31" t="s">
+        <v>435</v>
+      </c>
+      <c r="AW2" s="31" t="s">
+        <v>439</v>
+      </c>
+      <c r="AX2" s="31" t="s">
+        <v>497</v>
+      </c>
+      <c r="AY2" s="31" t="s">
+        <v>498</v>
+      </c>
+      <c r="AZ2" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA2" s="31" t="s">
+        <v>405</v>
+      </c>
+      <c r="BB2" s="31" t="s">
+        <v>485</v>
+      </c>
+      <c r="BC2" s="36"/>
+      <c r="BD2" s="25" t="s">
+        <v>461</v>
+      </c>
+      <c r="BE2" s="26" t="s">
+        <v>462</v>
+      </c>
+      <c r="BF2" s="27" t="s">
+        <v>417</v>
+      </c>
+      <c r="BG2" s="28" t="s">
+        <v>457</v>
+      </c>
+      <c r="BH2" s="26" t="s">
+        <v>463</v>
+      </c>
+      <c r="BI2" s="26" t="s">
+        <v>464</v>
+      </c>
+      <c r="BJ2" s="26" t="s">
+        <v>465</v>
+      </c>
+      <c r="BK2" s="27" t="s">
+        <v>418</v>
+      </c>
+      <c r="BL2" s="28" t="s">
+        <v>458</v>
+      </c>
+      <c r="BM2" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="BN2" s="29" t="s">
+        <v>467</v>
+      </c>
+      <c r="BO2" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="BP2" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="BQ2" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="BR2" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="BS2" s="28" t="s">
+        <v>460</v>
+      </c>
+      <c r="BT2" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="BU2" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="BV2" s="25" t="s">
+        <v>473</v>
+      </c>
+      <c r="BW2" s="25" t="s">
+        <v>474</v>
+      </c>
+      <c r="BX2" s="25" t="s">
+        <v>475</v>
+      </c>
+      <c r="BY2" s="25" t="s">
+        <v>476</v>
+      </c>
+      <c r="BZ2" s="25" t="s">
+        <v>477</v>
+      </c>
+      <c r="CA2" s="25" t="s">
+        <v>478</v>
+      </c>
+      <c r="CB2" s="25" t="s">
+        <v>479</v>
+      </c>
+      <c r="CC2" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="CD2" s="38" t="s">
+        <v>277</v>
+      </c>
+      <c r="CE2" s="38" t="s">
+        <v>278</v>
+      </c>
+      <c r="CF2" s="38" t="s">
+        <v>279</v>
+      </c>
+      <c r="CG2" s="38" t="s">
+        <v>280</v>
+      </c>
+      <c r="CH2" s="38" t="s">
+        <v>281</v>
+      </c>
+      <c r="CI2" s="38" t="s">
+        <v>282</v>
+      </c>
+      <c r="CJ2" s="38" t="s">
+        <v>283</v>
+      </c>
+      <c r="CK2" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="CL2" s="38" t="s">
         <v>285</v>
       </c>
-      <c r="K1" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="L1" s="19" t="s">
-        <v>425</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>357</v>
-      </c>
-      <c r="N1" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="19" t="s">
-        <v>328</v>
-      </c>
-      <c r="P1" s="19" t="s">
-        <v>327</v>
-      </c>
-      <c r="Q1" s="19" t="s">
-        <v>446</v>
-      </c>
-      <c r="R1" s="19" t="s">
-        <v>445</v>
-      </c>
-      <c r="S1" s="19" t="s">
-        <v>434</v>
-      </c>
-      <c r="T1" s="19" t="s">
-        <v>366</v>
-      </c>
-      <c r="U1" s="19" t="s">
-        <v>395</v>
-      </c>
-      <c r="V1" s="19" t="s">
-        <v>364</v>
-      </c>
-      <c r="W1" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="X1" s="19" t="s">
-        <v>351</v>
-      </c>
-      <c r="Y1" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="Z1" s="19" t="s">
-        <v>450</v>
-      </c>
-      <c r="AA1" s="19" t="s">
-        <v>276</v>
-      </c>
-      <c r="AB1" s="19" t="s">
-        <v>277</v>
-      </c>
-      <c r="AC1" s="19" t="s">
-        <v>329</v>
-      </c>
-      <c r="AD1" s="19" t="s">
-        <v>354</v>
-      </c>
-      <c r="AE1" s="19" t="s">
-        <v>369</v>
-      </c>
-      <c r="AF1" s="19" t="s">
-        <v>370</v>
-      </c>
-      <c r="AG1" s="19" t="s">
-        <v>371</v>
-      </c>
-      <c r="AH1" s="19" t="s">
-        <v>402</v>
-      </c>
-      <c r="AI1" s="19" t="s">
-        <v>374</v>
-      </c>
-      <c r="AJ1" s="19" t="s">
-        <v>389</v>
-      </c>
-      <c r="AK1" s="19" t="s">
-        <v>454</v>
-      </c>
-      <c r="AL1" s="19" t="s">
-        <v>355</v>
-      </c>
-      <c r="AM1" s="19" t="s">
-        <v>356</v>
-      </c>
-      <c r="AN1" s="19" t="s">
-        <v>278</v>
-      </c>
-      <c r="AO1" s="19" t="s">
-        <v>440</v>
-      </c>
-      <c r="AP1" s="19" t="s">
-        <v>279</v>
-      </c>
-      <c r="AQ1" s="21" t="s">
-        <v>330</v>
-      </c>
-      <c r="AR1" s="21" t="s">
-        <v>331</v>
-      </c>
-      <c r="AS1" s="21" t="s">
-        <v>332</v>
-      </c>
-      <c r="AT1" s="21" t="s">
-        <v>333</v>
-      </c>
-      <c r="AU1" s="21" t="s">
-        <v>334</v>
-      </c>
-      <c r="AV1" s="21" t="s">
-        <v>335</v>
-      </c>
-      <c r="AW1" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="AX1" s="22" t="s">
-        <v>337</v>
-      </c>
-      <c r="AY1" s="22" t="s">
-        <v>338</v>
-      </c>
-      <c r="AZ1" s="22" t="s">
-        <v>339</v>
-      </c>
-      <c r="BA1" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="BB1" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="BC1" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="BD1" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="BE1" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="BF1" s="20" t="s">
-        <v>284</v>
-      </c>
-      <c r="BG1" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="BH1" s="20" t="s">
+      <c r="CM2" s="38" t="s">
         <v>286</v>
       </c>
-      <c r="BI1" s="20" t="s">
+      <c r="CN2" s="38" t="s">
         <v>287</v>
       </c>
-      <c r="BJ1" s="20" t="s">
+      <c r="CO2" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="BK1" s="20" t="s">
+      <c r="CP2" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="BL1" s="20" t="s">
+      <c r="CQ2" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="BM1" s="20" t="s">
+      <c r="CR2" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="BN1" s="20" t="s">
+      <c r="CS2" s="38" t="s">
         <v>292</v>
       </c>
-      <c r="BO1" s="20" t="s">
+      <c r="CT2" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="BP1" s="20" t="s">
+      <c r="CU2" s="38" t="s">
         <v>294</v>
       </c>
-      <c r="BQ1" s="20" t="s">
+      <c r="CV2" s="38" t="s">
         <v>295</v>
       </c>
-      <c r="BR1" s="20" t="s">
+      <c r="CW2" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="BS1" s="20" t="s">
+      <c r="CX2" s="38" t="s">
         <v>297</v>
       </c>
-      <c r="BT1" s="20" t="s">
+      <c r="CY2" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="BU1" s="20" t="s">
+      <c r="CZ2" s="38" t="s">
         <v>299</v>
       </c>
-      <c r="BV1" s="20" t="s">
+      <c r="DA2" s="38" t="s">
         <v>300</v>
       </c>
-      <c r="BW1" s="20" t="s">
+      <c r="DB2" s="38" t="s">
         <v>301</v>
       </c>
-      <c r="BX1" s="20" t="s">
+      <c r="DC2" s="38" t="s">
         <v>302</v>
       </c>
-      <c r="BY1" s="20" t="s">
+    </row>
+    <row r="3" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="BZ1" s="20" t="s">
+      <c r="C3" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="CA1" s="20" t="s">
+      <c r="E3" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="2" spans="1:79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="3">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>409</v>
-      </c>
-      <c r="H2" s="13">
-        <v>2018</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>431</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="3">
-        <v>716</v>
-      </c>
-      <c r="Q2" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="Z2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="AC2" s="13">
-        <v>10</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="AF2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AG2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AH2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AI2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AJ2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AK2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AL2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AM2" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="AO2" s="13"/>
-      <c r="AP2" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="3" spans="1:79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E3" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>319</v>
-      </c>
       <c r="G3" s="13" t="s">
-        <v>409</v>
+        <v>380</v>
       </c>
       <c r="H3" s="13">
         <v>2018</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>410</v>
+        <v>35</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>312</v>
+        <v>161</v>
       </c>
       <c r="L3" s="13" t="s">
-        <v>430</v>
-      </c>
-      <c r="M3" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="N3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>24</v>
+      <c r="O3" s="13" t="s">
+        <v>305</v>
       </c>
       <c r="P3" s="3">
-        <v>819.95100000000002</v>
-      </c>
-      <c r="Q3" s="13" t="s">
-        <v>447</v>
-      </c>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13">
-        <v>245.98599999999999</v>
-      </c>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
+        <v>716</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="S3" s="13"/>
+      <c r="T3" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>339</v>
+      </c>
       <c r="V3" s="13"/>
-      <c r="W3" s="3" t="s">
-        <v>321</v>
+      <c r="W3" s="13" t="s">
+        <v>341</v>
       </c>
       <c r="X3" s="13"/>
       <c r="Y3" s="3" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="Z3" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB3" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="AA3" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="AB3" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="3" t="s">
-        <v>376</v>
+      <c r="AC3" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>305</v>
       </c>
       <c r="AE3" s="13"/>
-      <c r="AF3" s="13"/>
-      <c r="AG3" s="13"/>
-      <c r="AH3" s="13"/>
+      <c r="AF3" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="AH3" s="13" t="s">
+        <v>346</v>
+      </c>
       <c r="AI3" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="AJ3" s="13"/>
+        <v>305</v>
+      </c>
+      <c r="AJ3" s="13" t="s">
+        <v>305</v>
+      </c>
       <c r="AK3" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="AL3" s="13"/>
-      <c r="AM3" s="13"/>
-      <c r="AN3" s="3" t="s">
-        <v>324</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="AL3" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AM3" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AN3" s="13"/>
       <c r="AO3" s="13"/>
-      <c r="AP3" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="AK4" s="8" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="5" spans="1:79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C5" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>347</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="AP3" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AQ3" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AR3" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="13"/>
+      <c r="AU3" s="13"/>
+      <c r="AV3" s="13"/>
+      <c r="AW3" s="13"/>
+      <c r="AX3" s="13"/>
+      <c r="AY3" s="13"/>
+      <c r="AZ3" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="BA3" s="13"/>
+      <c r="BB3" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="BC3" s="13" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>428</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="H4" s="13">
+        <v>2018</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>381</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="P4" s="3">
+        <v>819.95100000000002</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="R4" s="13"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U4" s="13"/>
+      <c r="V4" s="13"/>
+      <c r="W4" s="13"/>
+      <c r="X4" s="13"/>
+      <c r="Y4" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="Z4" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AA4" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="AC4" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="13"/>
+      <c r="AF4" s="13">
+        <v>245.98599999999999</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AQ4" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AR4" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+      <c r="AW4" s="13"/>
+      <c r="AX4" s="13"/>
+      <c r="AY4" s="13"/>
+      <c r="AZ4" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="BA4" s="13"/>
+      <c r="BB4" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="BC4" s="13" t="s">
         <v>319</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="H5">
+    </row>
+    <row r="5" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AP5" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AQ5" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AR5" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AS5" s="8"/>
+      <c r="AT5" s="8"/>
+      <c r="AU5" s="8"/>
+      <c r="AV5" s="8"/>
+      <c r="AW5" s="8"/>
+      <c r="AX5" s="8"/>
+      <c r="AY5" s="8"/>
+    </row>
+    <row r="6" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="H6">
         <v>2015</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>411</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>429</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>359</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>358</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>360</v>
-      </c>
-      <c r="P5">
-        <v>59</v>
-      </c>
-      <c r="Q5" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="W5" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="X5" s="8" t="s">
-        <v>352</v>
-      </c>
-      <c r="Y5" s="8" t="s">
-        <v>353</v>
-      </c>
-      <c r="Z5" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AA5" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="AB5" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="AC5" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AD5" s="8" t="s">
-        <v>399</v>
-      </c>
-      <c r="AE5" s="8" t="s">
-        <v>377</v>
-      </c>
-      <c r="AF5" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="AG5" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="AH5" s="8"/>
-      <c r="AI5" s="8"/>
-      <c r="AJ5" s="8"/>
-      <c r="AK5" s="8"/>
-      <c r="AL5" s="8" t="s">
-        <v>380</v>
-      </c>
-      <c r="AM5" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="AP5" s="24" t="s">
+      <c r="I6" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="6" spans="1:79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D6" s="25" t="s">
-        <v>417</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="H6">
-        <v>2017</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>412</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>161</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>428</v>
+        <v>395</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>361</v>
+        <v>333</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>51</v>
+        <v>358</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>386</v>
+        <v>305</v>
       </c>
       <c r="P6">
-        <v>986</v>
+        <v>59</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>447</v>
+        <v>328</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="S6" s="8" t="s">
-        <v>310</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="S6" s="8"/>
       <c r="T6" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8" t="s">
-        <v>367</v>
-      </c>
-      <c r="W6" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="X6" s="8" t="s">
-        <v>310</v>
+        <v>334</v>
       </c>
       <c r="Y6" s="8" t="s">
-        <v>388</v>
+        <v>331</v>
       </c>
       <c r="Z6" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="AA6" s="13" t="s">
-        <v>400</v>
+        <v>342</v>
+      </c>
+      <c r="AB6" s="8" t="s">
+        <v>327</v>
       </c>
       <c r="AC6" s="8" t="s">
-        <v>310</v>
+        <v>410</v>
       </c>
       <c r="AD6" s="8" t="s">
-        <v>391</v>
+        <v>305</v>
       </c>
       <c r="AE6" s="8"/>
       <c r="AF6" s="8" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="AG6" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AH6" s="8"/>
+        <v>370</v>
+      </c>
+      <c r="AH6" s="8" t="s">
+        <v>351</v>
+      </c>
       <c r="AI6" s="8" t="s">
-        <v>310</v>
+        <v>353</v>
       </c>
       <c r="AJ6" s="8" t="s">
-        <v>390</v>
-      </c>
-      <c r="AK6" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AL6" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AM6" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AO6" s="8" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="7" spans="1:79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D7" s="25" t="s">
-        <v>416</v>
+        <v>352</v>
+      </c>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
+      <c r="AN6" s="8"/>
+      <c r="AO6" s="8"/>
+      <c r="AP6" s="8"/>
+      <c r="AQ6" s="8"/>
+      <c r="AR6" s="8"/>
+      <c r="AS6" s="8"/>
+      <c r="AT6" s="8"/>
+      <c r="AU6" s="8"/>
+      <c r="AV6" s="8"/>
+      <c r="AW6" s="8"/>
+      <c r="AX6" s="8"/>
+      <c r="AY6" s="8"/>
+      <c r="BB6" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="BC6" s="19" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>386</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>392</v>
+        <v>422</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="G7" s="26"/>
+        <v>313</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>380</v>
+      </c>
       <c r="H7">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="I7" s="8" t="s">
         <v>393</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>35</v>
+        <v>455</v>
       </c>
       <c r="K7" s="8" t="s">
         <v>161</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>426</v>
+        <v>394</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>361</v>
+        <v>51</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>51</v>
+        <v>358</v>
       </c>
       <c r="O7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="P7">
+        <v>986</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8" t="s">
+        <v>360</v>
+      </c>
+      <c r="Z7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AA7" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="AC7" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AG7" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AJ7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AM7" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="AN7" s="8"/>
+      <c r="AO7" s="8"/>
+      <c r="AP7" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AQ7" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AR7" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AS7" s="8"/>
+      <c r="AT7" s="8"/>
+      <c r="AU7" s="8"/>
+      <c r="AV7" s="8"/>
+      <c r="AW7" s="8"/>
+      <c r="AX7" s="8"/>
+      <c r="AY7" s="8"/>
+      <c r="BA7" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="BB7" s="8" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="8" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="P7">
-        <v>5</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="S7" s="8">
-        <v>5</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>394</v>
-      </c>
-      <c r="U7" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="W7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="X7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="Y7" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="Z7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AA7" s="8" t="s">
-        <v>368</v>
-      </c>
-      <c r="AB7" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="AC7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AD7" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="AE7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AF7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AG7" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="AH7" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="AI7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AJ7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AK7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AL7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AM7" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AN7" s="8" t="s">
-        <v>405</v>
-      </c>
-      <c r="AO7" s="8" t="s">
-        <v>406</v>
-      </c>
-      <c r="AP7" s="24" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="8" spans="1:79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D8" s="8" t="s">
-        <v>418</v>
+      <c r="D8" s="20" t="s">
+        <v>385</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>409</v>
-      </c>
+        <v>313</v>
+      </c>
+      <c r="G8" s="21"/>
       <c r="H8">
         <v>2015</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>414</v>
+        <v>364</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>415</v>
+        <v>35</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>161</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>426</v>
+        <v>392</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>361</v>
+        <v>51</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>419</v>
+        <v>358</v>
       </c>
       <c r="O8" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="P8">
+        <v>10</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="S8" s="8"/>
+      <c r="T8" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="V8" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="W8" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="Z8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AA8" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB8" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="AC8" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8">
+        <v>5</v>
+      </c>
+      <c r="AG8" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="AH8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AI8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AJ8" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="AK8" s="8" t="s">
+        <v>374</v>
+      </c>
+      <c r="AL8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AM8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AQ8" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AR8" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AS8" s="8"/>
+      <c r="AT8" s="8"/>
+      <c r="AU8" s="8"/>
+      <c r="AV8" s="8"/>
+      <c r="AW8" s="8"/>
+      <c r="AX8" s="8"/>
+      <c r="AY8" s="8"/>
+      <c r="AZ8" s="8" t="s">
+        <v>376</v>
+      </c>
+      <c r="BA8" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="BB8" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="BC8" s="19" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="9" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>387</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="P8">
-        <v>14</v>
-      </c>
-      <c r="Q8" s="8" t="s">
-        <v>447</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="S8" s="8">
-        <v>14</v>
-      </c>
-      <c r="T8" s="8" t="s">
-        <v>421</v>
-      </c>
-      <c r="U8" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="V8" s="8" t="s">
-        <v>421</v>
-      </c>
-      <c r="W8" s="8" t="s">
-        <v>423</v>
-      </c>
-      <c r="X8" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="Y8" s="8" t="s">
-        <v>433</v>
-      </c>
-      <c r="Z8" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AA8" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="AB8" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="AC8" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AD8" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="AE8" s="8" t="s">
-        <v>436</v>
-      </c>
-      <c r="AF8" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="AG8" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="AH8" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AI8" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="AJ8" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AK8" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AL8" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AM8" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AN8" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="AO8" s="25" t="s">
-        <v>439</v>
-      </c>
-      <c r="AP8" s="27" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="9" spans="1:79" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D9" s="8" t="s">
-        <v>456</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>457</v>
-      </c>
       <c r="F9" s="8" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>409</v>
+        <v>380</v>
+      </c>
+      <c r="H9">
+        <v>2015</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>443</v>
+        <v>383</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>442</v>
+        <v>384</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>161</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>426</v>
+        <v>392</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>359</v>
+        <v>388</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>444</v>
+        <v>358</v>
       </c>
       <c r="O9" s="8" t="s">
-        <v>458</v>
+        <v>489</v>
       </c>
       <c r="P9">
+        <v>28</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>391</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="Z9" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AA9" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB9" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="AC9" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD9" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8">
+        <v>14</v>
+      </c>
+      <c r="AG9" s="8" t="s">
+        <v>400</v>
+      </c>
+      <c r="AH9" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="AI9" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="AJ9" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="AK9" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AL9" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="AM9" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AN9" s="8"/>
+      <c r="AO9" s="8"/>
+      <c r="AP9" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AQ9" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AR9" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AS9" s="8"/>
+      <c r="AT9" s="8"/>
+      <c r="AU9" s="8"/>
+      <c r="AV9" s="8"/>
+      <c r="AW9" s="8"/>
+      <c r="AX9" s="8"/>
+      <c r="AY9" s="8"/>
+      <c r="AZ9" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="BA9" s="20" t="s">
+        <v>404</v>
+      </c>
+      <c r="BB9" s="20" t="s">
+        <v>410</v>
+      </c>
+      <c r="BC9" s="21" t="s">
+        <v>406</v>
+      </c>
+      <c r="BD9" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="BM9" s="21"/>
+      <c r="BN9" s="21"/>
+      <c r="BO9" s="21"/>
+      <c r="BP9" s="21"/>
+      <c r="BQ9" s="21"/>
+      <c r="BR9" s="21"/>
+      <c r="BS9" s="21"/>
+      <c r="BT9" s="21"/>
+      <c r="BU9" s="21"/>
+      <c r="BV9" s="21"/>
+      <c r="BW9" s="21"/>
+      <c r="BX9" s="21"/>
+      <c r="BY9" s="21"/>
+      <c r="BZ9" s="21"/>
+      <c r="CA9" s="21"/>
+      <c r="CB9" s="21"/>
+      <c r="CC9" s="21"/>
+    </row>
+    <row r="10" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="H10">
+        <v>2016</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="P10">
         <v>181</v>
       </c>
-      <c r="Q9" s="8" t="s">
+      <c r="Q10" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="R10" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="S10" s="22"/>
+      <c r="T10" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="W10" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="X10" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="Y10" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="Z10" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA10" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB10" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="AC10" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="AD10" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="AE10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF10">
+        <v>88</v>
+      </c>
+      <c r="AG10" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="AH10" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="AI10" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="AJ10" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="AK10" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AL10" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="AM10" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AN10" s="8"/>
+      <c r="AO10" s="8"/>
+      <c r="AP10" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="AQ10" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="AR10" s="8" t="s">
+        <v>434</v>
+      </c>
+      <c r="AS10" s="8"/>
+      <c r="AT10" s="8"/>
+      <c r="AU10" s="8"/>
+      <c r="AV10" s="8"/>
+      <c r="AW10" s="8"/>
+      <c r="AX10" s="8"/>
+      <c r="AY10" s="8"/>
+      <c r="BE10" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF10" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="BG10" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="BH10" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="BI10" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="BJ10" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="BK10" s="21" t="s">
+        <v>456</v>
+      </c>
+      <c r="BL10" s="21" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:107" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>420</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>380</v>
       </c>
-      <c r="R9" s="8" t="s">
-        <v>448</v>
-      </c>
-      <c r="S9">
-        <v>88</v>
-      </c>
-      <c r="T9" s="8" t="s">
-        <v>421</v>
-      </c>
-      <c r="V9" s="8" t="s">
-        <v>421</v>
-      </c>
-      <c r="W9" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="X9" s="28" t="s">
-        <v>449</v>
-      </c>
-      <c r="Y9" s="8" t="s">
+      <c r="H11">
+        <v>2015</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>443</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>489</v>
+      </c>
+      <c r="P11">
+        <v>296</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="R11" s="22" t="s">
+        <v>490</v>
+      </c>
+      <c r="S11" s="22"/>
+      <c r="T11" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="W11" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="Z9" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="AA9" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="AB9" s="8" t="s">
+      <c r="X11" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="Y11" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="Z11" s="8" t="s">
+        <v>412</v>
+      </c>
+      <c r="AA11" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="AB11" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="AC11" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AE11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AF11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AG11" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="AH11" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="AI11" s="8" t="s">
         <v>349</v>
       </c>
-      <c r="AC9" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AD9" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="AE9" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="AF9" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AG9" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AH9" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AI9" s="8" t="s">
-        <v>453</v>
-      </c>
-      <c r="AJ9" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AK9" s="8" t="s">
-        <v>455</v>
-      </c>
-      <c r="AL9" s="8" t="s">
-        <v>310</v>
-      </c>
-      <c r="AM9" s="8" t="s">
-        <v>310</v>
+      <c r="AJ11" s="8" t="s">
+        <v>494</v>
+      </c>
+      <c r="AK11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AL11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AM11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AN11" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="AO11" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="AP11" s="13" t="s">
+        <v>410</v>
+      </c>
+      <c r="AQ11" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="AR11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AS11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AT11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AU11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AV11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AW11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AX11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AY11" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="AZ11" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="BA11" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="BB11" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="BC11" s="18" t="s">
+        <v>503</v>
+      </c>
+      <c r="BE11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BF11" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="BG11" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="BH11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BI11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BJ11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BK11" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="BL11" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="BM11" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="BN11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BO11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BP11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BQ11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BR11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BS11" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="BT11" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="BU11" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="BV11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BW11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BX11" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="BY11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="BZ11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="CA11" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="CB11" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="CC11" s="8" t="s">
+        <v>510</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:BA1"/>
+    <mergeCell ref="BD1:CC1"/>
+    <mergeCell ref="CD1:DC1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="BC11" r:id="rId1" xr:uid="{2E588990-E6DC-244F-8579-F44F45514AD3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>